<commit_message>
Done thống keeee hú deeeeeeeeeeeeee
</commit_message>
<xml_diff>
--- a/src/ThongKeNhaHangERROR.xlsx
+++ b/src/ThongKeNhaHangERROR.xlsx
@@ -71,13 +71,13 @@
     <t>Tháng 12</t>
   </si>
   <si>
+    <t>220000</t>
+  </si>
+  <si>
     <t>HÔM NAY</t>
   </si>
   <si>
     <t>TUẦN</t>
-  </si>
-  <si>
-    <t>1172</t>
   </si>
   <si>
     <t>THÁNG</t>
@@ -224,16 +224,16 @@
     </row>
     <row r="4">
       <c r="C4" t="s" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E4" t="n" s="2">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F4" t="n" s="2">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G4" t="n" s="2">
         <v>0.0</v>
@@ -241,19 +241,19 @@
     </row>
     <row r="5">
       <c r="C5" t="s" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E5" t="n" s="2">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="F5" t="n" s="2">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="G5" t="n" s="2">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="6">
@@ -261,16 +261,16 @@
         <v>22</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E6" t="n" s="2">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="F6" t="n" s="2">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="G6" t="n" s="2">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="7">
@@ -278,16 +278,16 @@
         <v>23</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E7" t="n" s="2">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="F7" t="n" s="2">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="G7" t="n" s="2">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="10">
@@ -385,7 +385,7 @@
         <v>18</v>
       </c>
       <c r="F16" t="s" s="2">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix bug update rank KH
</commit_message>
<xml_diff>
--- a/src/ThongKeNhaHangERROR.xlsx
+++ b/src/ThongKeNhaHangERROR.xlsx
@@ -71,7 +71,7 @@
     <t>Tháng 12</t>
   </si>
   <si>
-    <t>220000</t>
+    <t>8536362</t>
   </si>
   <si>
     <t>HÔM NAY</t>
@@ -230,10 +230,10 @@
         <v>19</v>
       </c>
       <c r="E4" t="n" s="2">
-        <v>1.0</v>
+        <v>13.0</v>
       </c>
       <c r="F4" t="n" s="2">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G4" t="n" s="2">
         <v>0.0</v>
@@ -247,10 +247,10 @@
         <v>19</v>
       </c>
       <c r="E5" t="n" s="2">
-        <v>1.0</v>
+        <v>13.0</v>
       </c>
       <c r="F5" t="n" s="2">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G5" t="n" s="2">
         <v>0.0</v>
@@ -264,10 +264,10 @@
         <v>19</v>
       </c>
       <c r="E6" t="n" s="2">
-        <v>1.0</v>
+        <v>13.0</v>
       </c>
       <c r="F6" t="n" s="2">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G6" t="n" s="2">
         <v>0.0</v>
@@ -281,10 +281,10 @@
         <v>19</v>
       </c>
       <c r="E7" t="n" s="2">
-        <v>1.0</v>
+        <v>13.0</v>
       </c>
       <c r="F7" t="n" s="2">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G7" t="n" s="2">
         <v>0.0</v>

</xml_diff>